<commit_message>
Added ability to skip row in excel reader
</commit_message>
<xml_diff>
--- a/tasks_reader/test_resources/test_tasks.xlsx
+++ b/tasks_reader/test_resources/test_tasks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1160" windowWidth="28160" windowHeight="16100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Cart calculation logic - Part 1</t>
+  </si>
+  <si>
+    <t>Some other tasks</t>
   </si>
 </sst>
 </file>
@@ -150,8 +153,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -434,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,22 +455,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -526,77 +532,98 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>13</v>
-      </c>
-      <c r="G7">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="E8">
+      <c r="E12">
         <v>13</v>
       </c>
-      <c r="F8">
+      <c r="F12">
         <v>20</v>
       </c>
-      <c r="G8">
+      <c r="G12">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="F9">
+      <c r="F13">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added monte carlo emulation
</commit_message>
<xml_diff>
--- a/tasks_reader/test_resources/test_tasks.xlsx
+++ b/tasks_reader/test_resources/test_tasks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1160" windowWidth="28160" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1100" windowWidth="28160" windowHeight="16100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>id</t>
   </si>
@@ -60,9 +60,6 @@
     <t>TASK-4</t>
   </si>
   <si>
-    <t>TASK-2,TASK-3</t>
-  </si>
-  <si>
     <t>TASK-5</t>
   </si>
   <si>
@@ -100,6 +97,12 @@
   </si>
   <si>
     <t>Some other tasks</t>
+  </si>
+  <si>
+    <t>TASK-2, TASK-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TASK-1  </t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,7 +459,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -483,7 +486,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -500,7 +503,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -517,10 +520,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -537,13 +540,13 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -551,10 +554,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -568,7 +571,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -588,10 +591,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>13</v>
@@ -605,16 +608,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13">
         <v>40</v>

</xml_diff>